<commit_message>
Added Progress Notes + Date Extraction from Text
</commit_message>
<xml_diff>
--- a/dataset/oral cancer data.xlsx
+++ b/dataset/oral cancer data.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aseblr-my.sharepoint.com/personal/bl_en_u4cse22138_bl_students_amrita_edu/Documents/My Projects/TSA/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80A9C061-A999-477F-9DB4-8B5C7740A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{80A9C061-A999-477F-9DB4-8B5C7740A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A68E26A-3633-F04D-BC3B-0FDCC4DC312D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C172CD14-F1D3-4F00-B5BF-254AB502EC7F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17340" xr2:uid="{C172CD14-F1D3-4F00-B5BF-254AB502EC7F}"/>
   </bookViews>
   <sheets>
     <sheet name="oral cancer data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -479,6 +495,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -956,9 +975,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1336,11 +1356,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A3E416-EADD-45BC-AF16-1AB23CA9DE11}">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="R1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="18" max="18" width="8.83203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1418,7 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
@@ -1417,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1469,7 +1495,7 @@
       <c r="Q2">
         <v>2</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="S2">
@@ -1494,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1546,7 +1572,7 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S3">
@@ -1571,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1623,7 +1649,7 @@
       <c r="Q4">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="S4">
@@ -1648,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1700,7 +1726,7 @@
       <c r="Q5">
         <v>1</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="2">
         <v>41795</v>
       </c>
       <c r="S5">
@@ -1725,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1777,7 +1803,7 @@
       <c r="Q6">
         <v>2</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="S6">
@@ -1802,7 +1828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1854,7 +1880,7 @@
       <c r="Q7">
         <v>2</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="S7">
@@ -1879,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1931,7 +1957,7 @@
       <c r="Q8">
         <v>2</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="2">
         <v>44143</v>
       </c>
       <c r="S8">
@@ -1956,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2008,7 +2034,7 @@
       <c r="Q9">
         <v>2</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S9">
@@ -2033,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2085,7 +2111,7 @@
       <c r="Q10">
         <v>1</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="2">
         <v>40580</v>
       </c>
       <c r="S10">
@@ -2110,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2162,7 +2188,7 @@
       <c r="Q11">
         <v>1</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="S11">
@@ -2187,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2239,7 +2265,7 @@
       <c r="Q12">
         <v>1</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="S12">
@@ -2264,7 +2290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2316,7 +2342,7 @@
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="S13">
@@ -2341,7 +2367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2393,7 +2419,7 @@
       <c r="Q14">
         <v>1</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="2">
         <v>41032</v>
       </c>
       <c r="S14">
@@ -2418,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2470,7 +2496,7 @@
       <c r="Q15">
         <v>1</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="2" t="s">
         <v>45</v>
       </c>
       <c r="S15">
@@ -2495,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2547,7 +2573,7 @@
       <c r="Q16">
         <v>2</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16" s="2">
         <v>41585</v>
       </c>
       <c r="S16">
@@ -2572,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2624,7 +2650,7 @@
       <c r="Q17">
         <v>2</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="S17">
@@ -2634,9 +2660,6 @@
         <v>26</v>
       </c>
       <c r="U17" t="s">
-        <v>26</v>
-      </c>
-      <c r="V17" t="s">
         <v>26</v>
       </c>
       <c r="W17" t="s">
@@ -2649,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2701,7 +2724,7 @@
       <c r="Q18">
         <v>2</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="2" t="s">
         <v>49</v>
       </c>
       <c r="S18">
@@ -2726,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2778,7 +2801,7 @@
       <c r="Q19">
         <v>2</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="S19">
@@ -2803,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2855,7 +2878,7 @@
       <c r="Q20">
         <v>2</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="2" t="s">
         <v>53</v>
       </c>
       <c r="S20">
@@ -2880,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2932,7 +2955,7 @@
       <c r="Q21">
         <v>2</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="2" t="s">
         <v>55</v>
       </c>
       <c r="S21">
@@ -2957,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3009,7 +3032,7 @@
       <c r="Q22">
         <v>2</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="S22">
@@ -3034,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3086,7 +3109,7 @@
       <c r="Q23">
         <v>2</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="2" t="s">
         <v>58</v>
       </c>
       <c r="S23">
@@ -3111,7 +3134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3163,7 +3186,7 @@
       <c r="Q24">
         <v>2</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="2" t="s">
         <v>59</v>
       </c>
       <c r="S24">
@@ -3188,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3240,7 +3263,7 @@
       <c r="Q25">
         <v>2</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25" s="2">
         <v>44168</v>
       </c>
       <c r="S25">
@@ -3265,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3317,7 +3340,7 @@
       <c r="Q26">
         <v>2</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26" s="2" t="s">
         <v>62</v>
       </c>
       <c r="S26">
@@ -3342,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3394,7 +3417,7 @@
       <c r="Q27">
         <v>2</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="2" t="s">
         <v>63</v>
       </c>
       <c r="S27">
@@ -3419,7 +3442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3471,7 +3494,7 @@
       <c r="Q28">
         <v>2</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R28" s="2">
         <v>40545</v>
       </c>
       <c r="S28">
@@ -3496,7 +3519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3548,7 +3571,7 @@
       <c r="Q29">
         <v>2</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29" s="2" t="s">
         <v>66</v>
       </c>
       <c r="S29">
@@ -3573,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3625,7 +3648,7 @@
       <c r="Q30">
         <v>2</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30" s="2" t="s">
         <v>67</v>
       </c>
       <c r="S30">
@@ -3650,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3702,7 +3725,7 @@
       <c r="Q31">
         <v>2</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R31" s="2" t="s">
         <v>68</v>
       </c>
       <c r="S31">
@@ -3727,7 +3750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3779,7 +3802,7 @@
       <c r="Q32">
         <v>2</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32" s="2">
         <v>42624</v>
       </c>
       <c r="S32">
@@ -3804,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3856,7 +3879,7 @@
       <c r="Q33">
         <v>2</v>
       </c>
-      <c r="R33" t="s">
+      <c r="R33" s="2" t="s">
         <v>70</v>
       </c>
       <c r="S33">
@@ -3881,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3933,7 +3956,7 @@
       <c r="Q34">
         <v>2</v>
       </c>
-      <c r="R34" s="1">
+      <c r="R34" s="2">
         <v>41793</v>
       </c>
       <c r="S34">
@@ -3958,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4010,7 +4033,7 @@
       <c r="Q35">
         <v>2</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R35" s="2" t="s">
         <v>72</v>
       </c>
       <c r="S35">
@@ -4035,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4087,7 +4110,7 @@
       <c r="Q36">
         <v>2</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R36" s="2">
         <v>42195</v>
       </c>
       <c r="S36">
@@ -4112,7 +4135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4164,7 +4187,7 @@
       <c r="Q37">
         <v>2</v>
       </c>
-      <c r="R37" t="s">
+      <c r="R37" s="2" t="s">
         <v>74</v>
       </c>
       <c r="S37">
@@ -4189,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4241,7 +4264,7 @@
       <c r="Q38">
         <v>2</v>
       </c>
-      <c r="R38" s="1">
+      <c r="R38" s="2">
         <v>41651</v>
       </c>
       <c r="S38">
@@ -4266,7 +4289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4318,7 +4341,7 @@
       <c r="Q39">
         <v>2</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R39" s="2" t="s">
         <v>76</v>
       </c>
       <c r="S39">
@@ -4343,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4395,7 +4418,7 @@
       <c r="Q40">
         <v>2</v>
       </c>
-      <c r="R40" t="s">
+      <c r="R40" s="2" t="s">
         <v>78</v>
       </c>
       <c r="S40">
@@ -4420,7 +4443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4472,7 +4495,7 @@
       <c r="Q41">
         <v>2</v>
       </c>
-      <c r="R41" s="1">
+      <c r="R41" s="2">
         <v>42372</v>
       </c>
       <c r="S41">
@@ -4497,7 +4520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4549,7 +4572,7 @@
       <c r="Q42">
         <v>2</v>
       </c>
-      <c r="R42" t="s">
+      <c r="R42" s="2" t="s">
         <v>81</v>
       </c>
       <c r="S42">
@@ -4574,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4626,7 +4649,7 @@
       <c r="Q43">
         <v>2</v>
       </c>
-      <c r="R43" s="1">
+      <c r="R43" s="2">
         <v>42768</v>
       </c>
       <c r="S43">
@@ -4651,7 +4674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4703,7 +4726,7 @@
       <c r="Q44">
         <v>2</v>
       </c>
-      <c r="R44" t="s">
+      <c r="R44" s="2" t="s">
         <v>84</v>
       </c>
       <c r="S44">
@@ -4728,7 +4751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4780,7 +4803,7 @@
       <c r="Q45">
         <v>2</v>
       </c>
-      <c r="R45" t="s">
+      <c r="R45" s="2" t="s">
         <v>86</v>
       </c>
       <c r="S45">
@@ -4805,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4857,7 +4880,7 @@
       <c r="Q46">
         <v>2</v>
       </c>
-      <c r="R46" t="s">
+      <c r="R46" s="2" t="s">
         <v>88</v>
       </c>
       <c r="S46">
@@ -4882,7 +4905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4934,7 +4957,7 @@
       <c r="Q47">
         <v>2</v>
       </c>
-      <c r="R47" t="s">
+      <c r="R47" s="2" t="s">
         <v>39</v>
       </c>
       <c r="S47">
@@ -4959,7 +4982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5011,7 +5034,7 @@
       <c r="Q48">
         <v>2</v>
       </c>
-      <c r="R48" s="1">
+      <c r="R48" s="2">
         <v>43283</v>
       </c>
       <c r="S48">
@@ -5036,7 +5059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5088,7 +5111,7 @@
       <c r="Q49">
         <v>2</v>
       </c>
-      <c r="R49" s="1">
+      <c r="R49" s="2">
         <v>42372</v>
       </c>
       <c r="S49">
@@ -5113,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5165,7 +5188,7 @@
       <c r="Q50">
         <v>2</v>
       </c>
-      <c r="R50" s="1">
+      <c r="R50" s="2">
         <v>44287</v>
       </c>
       <c r="S50">
@@ -5190,7 +5213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5242,7 +5265,7 @@
       <c r="Q51">
         <v>2</v>
       </c>
-      <c r="R51" t="s">
+      <c r="R51" s="2" t="s">
         <v>91</v>
       </c>
       <c r="S51">
@@ -5267,7 +5290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5319,7 +5342,7 @@
       <c r="Q52">
         <v>2</v>
       </c>
-      <c r="R52" t="s">
+      <c r="R52" s="2" t="s">
         <v>93</v>
       </c>
       <c r="S52">
@@ -5344,7 +5367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5396,7 +5419,7 @@
       <c r="Q53">
         <v>2</v>
       </c>
-      <c r="R53" t="s">
+      <c r="R53" s="2" t="s">
         <v>94</v>
       </c>
       <c r="S53">
@@ -5421,7 +5444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5473,7 +5496,7 @@
       <c r="Q54">
         <v>2</v>
       </c>
-      <c r="R54" t="s">
+      <c r="R54" s="2" t="s">
         <v>96</v>
       </c>
       <c r="S54">
@@ -5498,7 +5521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5550,7 +5573,7 @@
       <c r="Q55">
         <v>2</v>
       </c>
-      <c r="R55" t="s">
+      <c r="R55" s="2" t="s">
         <v>97</v>
       </c>
       <c r="S55">
@@ -5575,7 +5598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5627,7 +5650,7 @@
       <c r="Q56">
         <v>2</v>
       </c>
-      <c r="R56" t="s">
+      <c r="R56" s="2" t="s">
         <v>100</v>
       </c>
       <c r="S56">
@@ -5652,7 +5675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5704,7 +5727,7 @@
       <c r="Q57">
         <v>2</v>
       </c>
-      <c r="R57" t="s">
+      <c r="R57" s="2" t="s">
         <v>101</v>
       </c>
       <c r="S57">
@@ -5729,7 +5752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5781,7 +5804,7 @@
       <c r="Q58">
         <v>2</v>
       </c>
-      <c r="R58" t="s">
+      <c r="R58" s="2" t="s">
         <v>103</v>
       </c>
       <c r="S58">
@@ -5806,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5858,7 +5881,7 @@
       <c r="Q59">
         <v>2</v>
       </c>
-      <c r="R59" s="1">
+      <c r="R59" s="2">
         <v>42193</v>
       </c>
       <c r="S59">
@@ -5883,7 +5906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5935,7 +5958,7 @@
       <c r="Q60">
         <v>2</v>
       </c>
-      <c r="R60" s="1">
+      <c r="R60" s="2">
         <v>43259</v>
       </c>
       <c r="S60">
@@ -5960,7 +5983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6012,7 +6035,7 @@
       <c r="Q61">
         <v>2</v>
       </c>
-      <c r="R61" t="s">
+      <c r="R61" s="2" t="s">
         <v>105</v>
       </c>
       <c r="S61">
@@ -6037,7 +6060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6089,7 +6112,7 @@
       <c r="Q62">
         <v>2</v>
       </c>
-      <c r="R62" s="1">
+      <c r="R62" s="2">
         <v>41345</v>
       </c>
       <c r="S62">
@@ -6114,7 +6137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6166,7 +6189,7 @@
       <c r="Q63">
         <v>2</v>
       </c>
-      <c r="R63" s="1">
+      <c r="R63" s="2">
         <v>42804</v>
       </c>
       <c r="S63">
@@ -6191,7 +6214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6243,7 +6266,7 @@
       <c r="Q64">
         <v>2</v>
       </c>
-      <c r="R64" s="1">
+      <c r="R64" s="2">
         <v>43415</v>
       </c>
       <c r="S64">
@@ -6268,7 +6291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6320,7 +6343,7 @@
       <c r="Q65">
         <v>2</v>
       </c>
-      <c r="R65" t="s">
+      <c r="R65" s="2" t="s">
         <v>109</v>
       </c>
       <c r="S65">
@@ -6345,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6397,7 +6420,7 @@
       <c r="Q66">
         <v>2</v>
       </c>
-      <c r="R66" t="s">
+      <c r="R66" s="2" t="s">
         <v>110</v>
       </c>
       <c r="S66">
@@ -6422,7 +6445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6474,7 +6497,7 @@
       <c r="Q67">
         <v>2</v>
       </c>
-      <c r="R67" t="s">
+      <c r="R67" s="2" t="s">
         <v>112</v>
       </c>
       <c r="S67">
@@ -6499,7 +6522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6551,7 +6574,7 @@
       <c r="Q68">
         <v>2</v>
       </c>
-      <c r="R68" t="s">
+      <c r="R68" s="2" t="s">
         <v>113</v>
       </c>
       <c r="S68">
@@ -6576,7 +6599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6628,7 +6651,7 @@
       <c r="Q69">
         <v>2</v>
       </c>
-      <c r="R69" s="1">
+      <c r="R69" s="2">
         <v>42378</v>
       </c>
       <c r="S69">
@@ -6653,7 +6676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6705,7 +6728,7 @@
       <c r="Q70">
         <v>2</v>
       </c>
-      <c r="R70" s="1">
+      <c r="R70" s="2">
         <v>43383</v>
       </c>
       <c r="S70">
@@ -6730,7 +6753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6782,7 +6805,7 @@
       <c r="Q71">
         <v>2</v>
       </c>
-      <c r="R71" s="1">
+      <c r="R71" s="2">
         <v>42100</v>
       </c>
       <c r="S71">
@@ -6807,7 +6830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6859,7 +6882,7 @@
       <c r="Q72">
         <v>2</v>
       </c>
-      <c r="R72" t="s">
+      <c r="R72" s="2" t="s">
         <v>115</v>
       </c>
       <c r="S72">
@@ -6884,7 +6907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6936,7 +6959,7 @@
       <c r="Q73">
         <v>2</v>
       </c>
-      <c r="R73" t="s">
+      <c r="R73" s="2" t="s">
         <v>117</v>
       </c>
       <c r="S73">
@@ -6961,7 +6984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7013,7 +7036,7 @@
       <c r="Q74">
         <v>2</v>
       </c>
-      <c r="R74" t="s">
+      <c r="R74" s="2" t="s">
         <v>118</v>
       </c>
       <c r="S74">
@@ -7038,7 +7061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -7090,7 +7113,7 @@
       <c r="Q75">
         <v>2</v>
       </c>
-      <c r="R75" t="s">
+      <c r="R75" s="2" t="s">
         <v>119</v>
       </c>
       <c r="S75">
@@ -7115,7 +7138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7167,7 +7190,7 @@
       <c r="Q76">
         <v>1</v>
       </c>
-      <c r="R76" s="1">
+      <c r="R76" s="2">
         <v>43624</v>
       </c>
       <c r="S76">
@@ -7192,7 +7215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7244,7 +7267,7 @@
       <c r="Q77">
         <v>1</v>
       </c>
-      <c r="R77" t="s">
+      <c r="R77" s="2" t="s">
         <v>122</v>
       </c>
       <c r="S77">
@@ -7269,7 +7292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7321,7 +7344,7 @@
       <c r="Q78">
         <v>1</v>
       </c>
-      <c r="R78" t="s">
+      <c r="R78" s="2" t="s">
         <v>123</v>
       </c>
       <c r="S78">
@@ -7346,7 +7369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7398,7 +7421,7 @@
       <c r="Q79">
         <v>1</v>
       </c>
-      <c r="R79" t="s">
+      <c r="R79" s="2" t="s">
         <v>124</v>
       </c>
       <c r="S79">
@@ -7423,7 +7446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7475,7 +7498,7 @@
       <c r="Q80">
         <v>1</v>
       </c>
-      <c r="R80" t="s">
+      <c r="R80" s="2" t="s">
         <v>126</v>
       </c>
       <c r="S80">
@@ -7500,7 +7523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7552,7 +7575,7 @@
       <c r="Q81">
         <v>1</v>
       </c>
-      <c r="R81" t="s">
+      <c r="R81" s="2" t="s">
         <v>128</v>
       </c>
       <c r="S81">
@@ -7577,7 +7600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7629,7 +7652,7 @@
       <c r="Q82">
         <v>1</v>
       </c>
-      <c r="R82" t="s">
+      <c r="R82" s="2" t="s">
         <v>130</v>
       </c>
       <c r="S82">
@@ -7654,7 +7677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7706,7 +7729,7 @@
       <c r="Q83">
         <v>1</v>
       </c>
-      <c r="R83" s="1">
+      <c r="R83" s="2">
         <v>41524</v>
       </c>
       <c r="S83">
@@ -7731,7 +7754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7783,7 +7806,7 @@
       <c r="Q84">
         <v>1</v>
       </c>
-      <c r="R84" t="s">
+      <c r="R84" s="2" t="s">
         <v>132</v>
       </c>
       <c r="S84">
@@ -7808,7 +7831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7860,7 +7883,7 @@
       <c r="Q85">
         <v>1</v>
       </c>
-      <c r="R85" t="s">
+      <c r="R85" s="2" t="s">
         <v>134</v>
       </c>
       <c r="S85">
@@ -7885,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7937,7 +7960,7 @@
       <c r="Q86">
         <v>1</v>
       </c>
-      <c r="R86" s="1">
+      <c r="R86" s="2">
         <v>41317</v>
       </c>
       <c r="S86">
@@ -7962,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -8014,7 +8037,7 @@
       <c r="Q87">
         <v>1</v>
       </c>
-      <c r="R87" s="1">
+      <c r="R87" s="2">
         <v>44502</v>
       </c>
       <c r="S87">
@@ -8039,7 +8062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8091,7 +8114,7 @@
       <c r="Q88">
         <v>1</v>
       </c>
-      <c r="R88" t="s">
+      <c r="R88" s="2" t="s">
         <v>136</v>
       </c>
       <c r="S88">
@@ -8116,7 +8139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8168,7 +8191,7 @@
       <c r="Q89">
         <v>1</v>
       </c>
-      <c r="R89" t="s">
+      <c r="R89" s="2" t="s">
         <v>138</v>
       </c>
       <c r="S89">
@@ -8193,7 +8216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8245,7 +8268,7 @@
       <c r="Q90">
         <v>1</v>
       </c>
-      <c r="R90" s="1">
+      <c r="R90" s="2">
         <v>41040</v>
       </c>
       <c r="S90">
@@ -8270,7 +8293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8322,7 +8345,7 @@
       <c r="Q91">
         <v>1</v>
       </c>
-      <c r="R91" t="s">
+      <c r="R91" s="2" t="s">
         <v>139</v>
       </c>
       <c r="S91">
@@ -8347,7 +8370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8399,7 +8422,7 @@
       <c r="Q92">
         <v>1</v>
       </c>
-      <c r="R92" t="s">
+      <c r="R92" s="2" t="s">
         <v>140</v>
       </c>
       <c r="S92">
@@ -8424,7 +8447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8476,7 +8499,7 @@
       <c r="Q93">
         <v>1</v>
       </c>
-      <c r="R93" s="1">
+      <c r="R93" s="2">
         <v>42258</v>
       </c>
       <c r="S93">
@@ -8501,7 +8524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8553,7 +8576,7 @@
       <c r="Q94">
         <v>1</v>
       </c>
-      <c r="R94" s="1">
+      <c r="R94" s="2">
         <v>43289</v>
       </c>
       <c r="S94">
@@ -8578,7 +8601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8630,7 +8653,7 @@
       <c r="Q95">
         <v>1</v>
       </c>
-      <c r="R95" t="s">
+      <c r="R95" s="2" t="s">
         <v>142</v>
       </c>
       <c r="S95">
@@ -8655,7 +8678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8707,7 +8730,7 @@
       <c r="Q96">
         <v>1</v>
       </c>
-      <c r="R96" t="s">
+      <c r="R96" s="2" t="s">
         <v>77</v>
       </c>
       <c r="S96">
@@ -8732,7 +8755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8784,7 +8807,7 @@
       <c r="Q97">
         <v>1</v>
       </c>
-      <c r="R97" t="s">
+      <c r="R97" s="2" t="s">
         <v>144</v>
       </c>
       <c r="S97">
@@ -8809,7 +8832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8861,7 +8884,7 @@
       <c r="Q98">
         <v>1</v>
       </c>
-      <c r="R98" s="1">
+      <c r="R98" s="2">
         <v>41465</v>
       </c>
       <c r="S98">
@@ -8886,7 +8909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8938,7 +8961,7 @@
       <c r="Q99">
         <v>1</v>
       </c>
-      <c r="R99" s="1">
+      <c r="R99" s="2">
         <v>41370</v>
       </c>
       <c r="S99">
@@ -8963,7 +8986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9015,7 +9038,7 @@
       <c r="Q100">
         <v>1</v>
       </c>
-      <c r="R100" t="s">
+      <c r="R100" s="2" t="s">
         <v>148</v>
       </c>
       <c r="S100">
@@ -9040,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9092,7 +9115,7 @@
       <c r="Q101">
         <v>1</v>
       </c>
-      <c r="R101" s="1">
+      <c r="R101" s="2">
         <v>42467</v>
       </c>
       <c r="S101">

</xml_diff>